<commit_message>
added the other results
</commit_message>
<xml_diff>
--- a/TOTAL_RESULTS_FILE.xlsx
+++ b/TOTAL_RESULTS_FILE.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kentmacdonald2/Documents/474-Trump-Classifier/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jvillama/Desktop/474-Trump-Classifier/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="22800" windowHeight="20020" tabRatio="500"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="13980" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="12">
   <si>
     <t>M-NB</t>
   </si>
@@ -51,6 +52,18 @@
   </si>
   <si>
     <t>F-Score</t>
+  </si>
+  <si>
+    <t>Trump vs Politicians, Unbalanced</t>
+  </si>
+  <si>
+    <t>Trump vs Politicians, BALANCED</t>
+  </si>
+  <si>
+    <t>Trump vs Obama, BALANCED</t>
+  </si>
+  <si>
+    <t>Trump vs Supporters, BALANCED</t>
   </si>
 </sst>
 </file>
@@ -349,11 +362,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1965343472"/>
-        <c:axId val="-1965341152"/>
+        <c:axId val="1185515072"/>
+        <c:axId val="1185517392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1965343472"/>
+        <c:axId val="1185515072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -388,7 +401,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1965341152"/>
+        <c:crossAx val="1185517392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -396,7 +409,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1965341152"/>
+        <c:axId val="1185517392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -429,7 +442,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1965343472"/>
+        <c:crossAx val="1185515072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -1405,8 +1418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1496,4 +1509,363 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.90817999999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.4995</v>
+      </c>
+      <c r="D3">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0.92181000000000002</v>
+      </c>
+      <c r="C4">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="D4">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0.90908999999999995</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>0.93606</v>
+      </c>
+      <c r="C6">
+        <v>0.73380000000000001</v>
+      </c>
+      <c r="D6">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>0.94</v>
+      </c>
+      <c r="C7">
+        <v>0.754</v>
+      </c>
+      <c r="D7">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>0.88533333333300002</v>
+      </c>
+      <c r="C11">
+        <v>0.88533333333300002</v>
+      </c>
+      <c r="D11">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0.89383333333299997</v>
+      </c>
+      <c r="C12">
+        <v>0.89383333333299997</v>
+      </c>
+      <c r="D12">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>0.50849999999999995</v>
+      </c>
+      <c r="C13">
+        <v>0.50849999999999995</v>
+      </c>
+      <c r="D13">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>0.84283333333300003</v>
+      </c>
+      <c r="C14">
+        <v>0.84283333333300003</v>
+      </c>
+      <c r="D14">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>0.87983333333299996</v>
+      </c>
+      <c r="C15">
+        <v>0.87983333333299996</v>
+      </c>
+      <c r="D15">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>0.98283333333300005</v>
+      </c>
+      <c r="C19">
+        <v>0.98283333333300005</v>
+      </c>
+      <c r="D19">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>0.98</v>
+      </c>
+      <c r="C20">
+        <v>0.98</v>
+      </c>
+      <c r="D20">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>0.567166666667</v>
+      </c>
+      <c r="C21">
+        <v>0.567166666667</v>
+      </c>
+      <c r="D21">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>0.95650000000000002</v>
+      </c>
+      <c r="C22">
+        <v>0.95650000000000002</v>
+      </c>
+      <c r="D22">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>0.97133333333299998</v>
+      </c>
+      <c r="C23">
+        <v>0.97133333333299998</v>
+      </c>
+      <c r="D23">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>0.83650000000000002</v>
+      </c>
+      <c r="C27">
+        <v>0.83650000000000002</v>
+      </c>
+      <c r="D27">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0.84233333333299998</v>
+      </c>
+      <c r="C28">
+        <v>0.84233333333299998</v>
+      </c>
+      <c r="D28">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>0.51349999999999996</v>
+      </c>
+      <c r="C29">
+        <v>0.51349999999999996</v>
+      </c>
+      <c r="D29">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>0.82683333333300002</v>
+      </c>
+      <c r="C30">
+        <v>0.82683333333300002</v>
+      </c>
+      <c r="D30">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>0.83733333333299997</v>
+      </c>
+      <c r="C31">
+        <v>0.83733333333299997</v>
+      </c>
+      <c r="D31">
+        <v>0.84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New representations of the results, and references in bibtex
</commit_message>
<xml_diff>
--- a/TOTAL_RESULTS_FILE.xlsx
+++ b/TOTAL_RESULTS_FILE.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kentmacdonald2/Documents/474-Trump-Classifier/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jvillama/Desktop/474-Trump-Classifier/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="29020" windowHeight="20440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="27940" windowHeight="17540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2 (Black)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,8 +28,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="O23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="12">
   <si>
     <t>M-NB</t>
   </si>
@@ -70,13 +103,24 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -362,11 +406,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1840801792"/>
-        <c:axId val="-1840799744"/>
+        <c:axId val="-391393280"/>
+        <c:axId val="-393143984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1840801792"/>
+        <c:axId val="-391393280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -401,7 +445,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1840799744"/>
+        <c:crossAx val="-393143984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -409,7 +453,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1840799744"/>
+        <c:axId val="-393143984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -442,7 +486,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1840801792"/>
+        <c:crossAx val="-391393280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -457,7 +501,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -766,11 +809,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1767664352"/>
-        <c:axId val="-1767662032"/>
+        <c:axId val="-393056352"/>
+        <c:axId val="-393053888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1767664352"/>
+        <c:axId val="-393056352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -805,7 +848,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1767662032"/>
+        <c:crossAx val="-393053888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -813,7 +856,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1767662032"/>
+        <c:axId val="-393053888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -846,7 +889,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1767664352"/>
+        <c:crossAx val="-393056352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -861,7 +904,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1170,11 +1212,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1767748912"/>
-        <c:axId val="-1767877248"/>
+        <c:axId val="-392983328"/>
+        <c:axId val="-392971776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1767748912"/>
+        <c:axId val="-392983328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1209,7 +1251,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1767877248"/>
+        <c:crossAx val="-392971776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1217,13 +1259,14 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1767877248"/>
+        <c:axId val="-392971776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1251,7 +1294,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1767748912"/>
+        <c:crossAx val="-392983328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -1266,7 +1309,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1575,11 +1617,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2006927568"/>
-        <c:axId val="-1843561360"/>
+        <c:axId val="-392902544"/>
+        <c:axId val="-392894272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2006927568"/>
+        <c:axId val="-392902544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1614,7 +1656,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1843561360"/>
+        <c:crossAx val="-392894272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1622,12 +1664,13 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1843561360"/>
+        <c:axId val="-392894272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1655,11 +1698,536 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2006927568"/>
+        <c:crossAx val="-392902544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Didact Gothic" charset="0"/>
+              <a:ea typeface="Didact Gothic" charset="0"/>
+              <a:cs typeface="Didact Gothic" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800">
+                <a:latin typeface="Didact Gothic" charset="0"/>
+                <a:ea typeface="Didact Gothic" charset="0"/>
+                <a:cs typeface="Didact Gothic" charset="0"/>
+              </a:rPr>
+              <a:t>Trump vs. Politicians</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet2 (Black)'!$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet2 (Black)'!$A$11:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>B-NB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>M-NB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SVM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>J48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SGD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet2 (Black)'!$B$11:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.885333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.893833333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5085</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.842833333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.879833333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet2 (Black)'!$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AUC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="E7E6E6">
+                <a:lumMod val="50000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet2 (Black)'!$A$11:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>B-NB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>M-NB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SVM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>J48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SGD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet2 (Black)'!$C$11:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.885333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.893833333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5085</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.842833333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.879833333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet2 (Black)'!$D$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>F-Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="E7E6E6">
+                <a:lumMod val="90000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet2 (Black)'!$A$11:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>B-NB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>M-NB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SVM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>J48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SGD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet2 (Black)'!$D$11:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-392803312"/>
+        <c:axId val="-392801136"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-392803312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Didact Gothic" charset="0"/>
+                <a:ea typeface="Didact Gothic" charset="0"/>
+                <a:cs typeface="Didact Gothic" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-392801136"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-392801136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Didact Gothic" charset="0"/>
+                <a:ea typeface="Didact Gothic" charset="0"/>
+                <a:cs typeface="Didact Gothic" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-392803312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln w="25400">
@@ -1686,7 +2254,1087 @@
           <a:pPr>
             <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="bg1"/>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Didact Gothic" charset="0"/>
+              <a:ea typeface="Didact Gothic" charset="0"/>
+              <a:cs typeface="Didact Gothic" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Didact Gothic" charset="0"/>
+                <a:ea typeface="Didact Gothic" charset="0"/>
+                <a:cs typeface="Didact Gothic" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800">
+                <a:latin typeface="Didact Gothic" charset="0"/>
+                <a:ea typeface="Didact Gothic" charset="0"/>
+                <a:cs typeface="Didact Gothic" charset="0"/>
+              </a:rPr>
+              <a:t>Trump</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="0">
+                <a:latin typeface="Didact Gothic" charset="0"/>
+                <a:ea typeface="Didact Gothic" charset="0"/>
+                <a:cs typeface="Didact Gothic" charset="0"/>
+              </a:rPr>
+              <a:t> vs. Obama</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800">
+              <a:latin typeface="Didact Gothic" charset="0"/>
+              <a:ea typeface="Didact Gothic" charset="0"/>
+              <a:cs typeface="Didact Gothic" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Didact Gothic" charset="0"/>
+              <a:ea typeface="Didact Gothic" charset="0"/>
+              <a:cs typeface="Didact Gothic" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet2 (Black)'!$B$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet2 (Black)'!$A$19:$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>B-NB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>M-NB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SVM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>J48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SGD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet2 (Black)'!$B$19:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.982833333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.567166666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9565</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.971333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet2 (Black)'!$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AUC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="E7E6E6">
+                <a:lumMod val="50000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet2 (Black)'!$A$19:$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>B-NB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>M-NB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SVM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>J48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SGD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet2 (Black)'!$C$19:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.982833333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.567166666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9565</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.971333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet2 (Black)'!$D$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>F-Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="E7E6E6">
+                <a:lumMod val="90000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet2 (Black)'!$A$19:$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>B-NB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>M-NB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SVM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>J48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SGD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet2 (Black)'!$D$19:$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-392735872"/>
+        <c:axId val="-392734096"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-392735872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Didact Gothic" charset="0"/>
+                <a:ea typeface="Didact Gothic" charset="0"/>
+                <a:cs typeface="Didact Gothic" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-392734096"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-392734096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Didact Gothic" charset="0"/>
+                <a:ea typeface="Didact Gothic" charset="0"/>
+                <a:cs typeface="Didact Gothic" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-392735872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Didact Gothic" charset="0"/>
+              <a:ea typeface="Didact Gothic" charset="0"/>
+              <a:cs typeface="Didact Gothic" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800">
+                <a:latin typeface="Didact Gothic" charset="0"/>
+                <a:ea typeface="Didact Gothic" charset="0"/>
+                <a:cs typeface="Didact Gothic" charset="0"/>
+              </a:rPr>
+              <a:t>Trump</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="0">
+                <a:latin typeface="Didact Gothic" charset="0"/>
+                <a:ea typeface="Didact Gothic" charset="0"/>
+                <a:cs typeface="Didact Gothic" charset="0"/>
+              </a:rPr>
+              <a:t> vs. Supporters</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800">
+              <a:latin typeface="Didact Gothic" charset="0"/>
+              <a:ea typeface="Didact Gothic" charset="0"/>
+              <a:cs typeface="Didact Gothic" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet2 (Black)'!$B$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet2 (Black)'!$A$27:$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>B-NB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>M-NB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SVM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>J48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SGD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet2 (Black)'!$B$27:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.8365</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.842333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5135</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.826833333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.837333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet2 (Black)'!$C$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AUC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="E7E6E6">
+                <a:lumMod val="50000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet2 (Black)'!$A$27:$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>B-NB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>M-NB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SVM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>J48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SGD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet2 (Black)'!$C$27:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.8365</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.842333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5135</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.826833333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.837333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet2 (Black)'!$D$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>F-Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="E7E6E6">
+                <a:lumMod val="90000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet2 (Black)'!$A$27:$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>B-NB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>M-NB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SVM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>J48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SGD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet2 (Black)'!$D$27:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-392675504"/>
+        <c:axId val="-392671632"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-392675504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Didact Gothic" charset="0"/>
+                <a:ea typeface="Didact Gothic" charset="0"/>
+                <a:cs typeface="Didact Gothic" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-392671632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-392671632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Didact Gothic" charset="0"/>
+                <a:ea typeface="Didact Gothic" charset="0"/>
+                <a:cs typeface="Didact Gothic" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-392675504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="Didact Gothic" charset="0"/>
               <a:ea typeface="Didact Gothic" charset="0"/>
@@ -1891,6 +3539,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3401,6 +5169,1515 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3999,16 +7276,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4017,7 +7294,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3581400" y="50800"/>
+          <a:off x="8534400" y="406400"/>
           <a:ext cx="6235700" cy="10045700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4131,6 +7408,107 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>427433</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>6899</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>423333</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>204494</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>514348</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>15210</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>403054</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>16228</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>411072</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>94617</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>269393</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>164857</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -5164,6 +8542,762 @@
 </a:themeOverride>
 </file>
 
+<file path=xl/theme/themeOverride4.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="Yu Gothic Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="DengXian Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="Yu Gothic"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="DengXian"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
+<file path=xl/theme/themeOverride5.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="Yu Gothic Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="DengXian Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="Yu Gothic"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="DengXian"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
+<file path=xl/theme/themeOverride6.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="Yu Gothic Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="DengXian Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="Yu Gothic"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="DengXian"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
@@ -5265,8 +9399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5617,6 +9751,369 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O31"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="66" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="O60" sqref="O60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.90817999999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.4995</v>
+      </c>
+      <c r="D3">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0.92181000000000002</v>
+      </c>
+      <c r="C4">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="D4">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0.90908999999999995</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>0.93606</v>
+      </c>
+      <c r="C6">
+        <v>0.73380000000000001</v>
+      </c>
+      <c r="D6">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>0.94</v>
+      </c>
+      <c r="C7">
+        <v>0.754</v>
+      </c>
+      <c r="D7">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>0.88533333333300002</v>
+      </c>
+      <c r="C11">
+        <v>0.88533333333300002</v>
+      </c>
+      <c r="D11">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0.89383333333299997</v>
+      </c>
+      <c r="C12">
+        <v>0.89383333333299997</v>
+      </c>
+      <c r="D12">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>0.50849999999999995</v>
+      </c>
+      <c r="C13">
+        <v>0.50849999999999995</v>
+      </c>
+      <c r="D13">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>0.84283333333300003</v>
+      </c>
+      <c r="C14">
+        <v>0.84283333333300003</v>
+      </c>
+      <c r="D14">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>0.87983333333299996</v>
+      </c>
+      <c r="C15">
+        <v>0.87983333333299996</v>
+      </c>
+      <c r="D15">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>0.98283333333300005</v>
+      </c>
+      <c r="C19">
+        <v>0.98283333333300005</v>
+      </c>
+      <c r="D19">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>0.98</v>
+      </c>
+      <c r="C20">
+        <v>0.98</v>
+      </c>
+      <c r="D20">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>0.567166666667</v>
+      </c>
+      <c r="C21">
+        <v>0.567166666667</v>
+      </c>
+      <c r="D21">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>0.95650000000000002</v>
+      </c>
+      <c r="C22">
+        <v>0.95650000000000002</v>
+      </c>
+      <c r="D22">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>0.97133333333299998</v>
+      </c>
+      <c r="C23">
+        <v>0.97133333333299998</v>
+      </c>
+      <c r="D23">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>0.83650000000000002</v>
+      </c>
+      <c r="C27">
+        <v>0.83650000000000002</v>
+      </c>
+      <c r="D27">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0.84233333333299998</v>
+      </c>
+      <c r="C28">
+        <v>0.84233333333299998</v>
+      </c>
+      <c r="D28">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>0.51349999999999996</v>
+      </c>
+      <c r="C29">
+        <v>0.51349999999999996</v>
+      </c>
+      <c r="D29">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>0.82683333333300002</v>
+      </c>
+      <c r="C30">
+        <v>0.82683333333300002</v>
+      </c>
+      <c r="D30">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>0.83733333333299997</v>
+      </c>
+      <c r="C31">
+        <v>0.83733333333299997</v>
+      </c>
+      <c r="D31">
+        <v>0.84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>